<commit_message>
pdf & excel program of RMC
</commit_message>
<xml_diff>
--- a/assets/RMCDirect-GrillleProgramme2017.xlsx
+++ b/assets/RMCDirect-GrillleProgramme2017.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="RMC Live - Grille du Programme du Direct" sheetId="1" state="visible" r:id="rId2"/>
@@ -206,7 +206,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -241,11 +241,6 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -326,7 +321,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -413,8 +408,8 @@
   </sheetPr>
   <dimension ref="B1:I25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="87" zoomScaleNormal="87" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -468,7 +463,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
@@ -490,7 +485,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
@@ -504,7 +499,7 @@
       </c>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
@@ -518,7 +513,7 @@
       </c>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="5" t="s">
         <v>15</v>
       </c>
@@ -532,7 +527,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="5" t="s">
         <v>16</v>
       </c>
@@ -546,7 +541,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="5" t="s">
         <v>17</v>
       </c>
@@ -568,7 +563,7 @@
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="5" t="s">
         <v>19</v>
       </c>
@@ -584,7 +579,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="5" t="s">
         <v>20</v>
       </c>
@@ -606,7 +601,7 @@
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="5" t="s">
         <v>22</v>
       </c>
@@ -620,7 +615,7 @@
       </c>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="5" t="s">
         <v>24</v>
       </c>
@@ -634,7 +629,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="5" t="s">
         <v>25</v>
       </c>
@@ -656,7 +651,7 @@
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="5" t="s">
         <v>27</v>
       </c>
@@ -672,7 +667,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="5" t="s">
         <v>30</v>
       </c>
@@ -694,7 +689,7 @@
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="5" t="s">
         <v>32</v>
       </c>
@@ -714,7 +709,7 @@
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="5" t="s">
         <v>34</v>
       </c>
@@ -732,7 +727,7 @@
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="5" t="s">
         <v>36</v>
       </c>
@@ -748,7 +743,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="5" t="s">
         <v>38</v>
       </c>
@@ -762,7 +757,7 @@
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="5" t="s">
         <v>39</v>
       </c>
@@ -780,7 +775,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="5" t="s">
         <v>43</v>
       </c>
@@ -794,7 +789,7 @@
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="5" t="s">
         <v>45</v>
       </c>
@@ -820,7 +815,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="5" t="s">
         <v>49</v>
       </c>
@@ -843,7 +838,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>